<commit_message>
ndimas profile provider, main page
</commit_message>
<xml_diff>
--- a/assets/data/address.xlsx
+++ b/assets/data/address.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew2\flutter_application_1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B00CBB7-7A40-497F-A5F3-2AF04B5D0274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D942B299-9060-4414-931E-4E1DE18E8611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -90,9 +90,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -373,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -386,7 +385,7 @@
     <col min="4" max="4" width="22.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -399,8 +398,14 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1">
+        <v>3.4996999999999998</v>
+      </c>
+      <c r="F1">
+        <v>98.9923</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -413,9 +418,15 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="E2">
+        <v>3.5861999999999998</v>
+      </c>
+      <c r="F2">
+        <v>98.600300000000004</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
@@ -426,9 +437,16 @@
       </c>
       <c r="D3" t="s">
         <v>9</v>
+      </c>
+      <c r="E3">
+        <v>4.1567999999999996</v>
+      </c>
+      <c r="F3">
+        <v>98.600499999999997</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ndimas add more orders v2
</commit_message>
<xml_diff>
--- a/assets/data/address.xlsx
+++ b/assets/data/address.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mikroskil\Sem4\Visual Studio Code\ProjectNew2\flutter_application_1\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C026FC9-C36B-4BB9-A373-4F0548E66099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A10342B8-FCB1-44FA-8363-D0071A381EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3156" yWindow="552" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,7 +378,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -403,10 +403,10 @@
         <v>2</v>
       </c>
       <c r="E1">
-        <v>3.4996999999999998</v>
+        <v>3.5697000000000001</v>
       </c>
       <c r="F1">
-        <v>98.9923</v>
+        <v>98.832300000000004</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -449,7 +449,7 @@
         <v>9</v>
       </c>
       <c r="E3">
-        <v>4.1567999999999996</v>
+        <v>3.6168</v>
       </c>
       <c r="F3">
         <v>98.600499999999997</v>

</xml_diff>